<commit_message>
docs thieu thi phai
</commit_message>
<xml_diff>
--- a/docs/Auction.xlsx
+++ b/docs/Auction.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t xml:space="preserve">Chức năng</t>
   </si>
@@ -131,19 +131,22 @@
     <t xml:space="preserve">Tạo vật đấu giá</t>
   </si>
   <si>
-    <t xml:space="preserve">ITEMADD [ItemName] [StartingBid] [BuyItNowPrice]</t>
+    <t xml:space="preserve">ITEMADD[ItemDetals][StartingBid][BuyItNowPrice]</t>
   </si>
   <si>
     <t xml:space="preserve">1070: add success</t>
   </si>
   <si>
-    <t xml:space="preserve">2071: Already have item</t>
+    <t xml:space="preserve">2071: Illogical Item Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2072: Waiting Room Full</t>
   </si>
   <si>
     <t xml:space="preserve">Xóa vật đấu giá</t>
   </si>
   <si>
-    <t xml:space="preserve">ITEMRETRIEVE [ItemName]</t>
+    <t xml:space="preserve">ITEMRETRIEVE[ID_ITEM]</t>
   </si>
   <si>
     <t xml:space="preserve">1080 : retrieve sucess</t>
@@ -155,13 +158,13 @@
     <t xml:space="preserve">2082: Nonexistent Item</t>
   </si>
   <si>
-    <t xml:space="preserve">2083: Not own this item</t>
+    <t xml:space="preserve">2083:  Invalid Input Format</t>
   </si>
   <si>
     <t xml:space="preserve">Tố giá </t>
   </si>
   <si>
-    <t xml:space="preserve">BID [ITEM_PRICE]</t>
+    <t xml:space="preserve">BID[ITEM_PRICE]</t>
   </si>
   <si>
     <t xml:space="preserve">1090: Successful Bid</t>
@@ -182,6 +185,9 @@
     <t xml:space="preserve">1100: Successful Buy</t>
   </si>
   <si>
+    <t xml:space="preserve">2101: Pre-existing Bidder</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sai ngữ pháp</t>
   </si>
   <si>
@@ -195,6 +201,18 @@
   </si>
   <si>
     <t xml:space="preserve">4092: Best price is </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dang ky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIGNUP [usename] [password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1110: Signup success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2111: Account already exist</t>
   </si>
 </sst>
 </file>
@@ -205,7 +223,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[h]:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -227,6 +245,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,7 +302,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -299,11 +323,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,21 +360,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -349,7 +384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -358,7 +393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -369,35 +404,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -408,35 +443,35 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -447,21 +482,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -472,14 +507,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="41.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -490,14 +525,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -508,33 +543,33 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -545,165 +580,202 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="2" t="s">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
       <c r="C36" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="2" t="s">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
       <c r="C41" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="6" t="s">
+      <c r="B45" s="6"/>
+      <c r="C45" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="6" t="s">
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="22">
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A8:A12"/>
@@ -716,18 +788,20 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>